<commit_message>
REVERT ALL COMMITS TO MASTER FOR 0.1.0 relesase
This commit fixes all changes that should have been kept in DEV for the
0.1.0 release
</commit_message>
<xml_diff>
--- a/python_tools/test/test_data/test_manifests/test_manifest_multilane.xlsx
+++ b/python_tools/test/test_data/test_manifests/test_manifest_multilane.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SampleInfo" sheetId="1" r:id="rId1"/>
@@ -252,13 +252,13 @@
     <t>test_sample_1_N</t>
   </si>
   <si>
+    <t>PROJECT_ID</t>
+  </si>
+  <si>
     <t>Test_Project_1</t>
   </si>
   <si>
     <t>Test_Project_2</t>
-  </si>
-  <si>
-    <t>STUDY_ID</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +696,7 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -856,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -936,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="Z4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -1016,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="Z5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1096,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="Z6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="Z7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>